<commit_message>
CP-159: Fixed Student template and Student Group template so they have the correct student info. Added stop-gap thread timer in SbossAutomationPreloader to wait for ART to calculate student to tests mappings.
</commit_message>
<xml_diff>
--- a/irp-automation-adapter-sboss-application/src/main/resources/irp-package/IRPStudents.xlsx
+++ b/irp-automation-adapter-sboss-application/src/main/resources/irp-package/IRPStudents.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="STUDENT" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="69">
   <si>
     <t>SSID</t>
   </si>
@@ -200,34 +200,40 @@
     <t>IRP39990002</t>
   </si>
   <si>
-    <t>IRP39990003</t>
-  </si>
-  <si>
-    <t>IRP39990004</t>
-  </si>
-  <si>
-    <t>IRP39990005</t>
-  </si>
-  <si>
-    <t>IRP39990006</t>
-  </si>
-  <si>
     <t>AIRP39990001</t>
   </si>
   <si>
     <t>AIRP39990002</t>
   </si>
   <si>
-    <t>AIRP39990003</t>
-  </si>
-  <si>
-    <t>AIRP39990004</t>
-  </si>
-  <si>
-    <t>AIRP39990005</t>
-  </si>
-  <si>
-    <t>AIRP39990006</t>
+    <t>07</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>IRP79990001</t>
+  </si>
+  <si>
+    <t>IRP79990002</t>
+  </si>
+  <si>
+    <t>IRP119990001</t>
+  </si>
+  <si>
+    <t>IRP119990002</t>
+  </si>
+  <si>
+    <t>AIRP119990001</t>
+  </si>
+  <si>
+    <t>AIRP119990002</t>
+  </si>
+  <si>
+    <t>AIRP79990001</t>
+  </si>
+  <si>
+    <t>AIRP79990002</t>
   </si>
 </sst>
 </file>
@@ -766,7 +772,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -915,7 +923,7 @@
         <v>55</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>34</v>
@@ -998,7 +1006,7 @@
         <v>56</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>34</v>
@@ -1078,13 +1086,13 @@
         <v>39510</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>7</v>
@@ -1161,13 +1169,13 @@
         <v>39511</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>7</v>
@@ -1250,13 +1258,13 @@
         <v>39512</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>65</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>5</v>
@@ -1333,13 +1341,13 @@
         <v>39513</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>66</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>5</v>
@@ -1399,7 +1407,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="J2 J3:J7" numberStoredAsText="1"/>
+    <ignoredError sqref="J2 J3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>